<commit_message>
working watershed summary excel file
</commit_message>
<xml_diff>
--- a/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
+++ b/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
@@ -9,8 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Estimated Runoff" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Water Rights Licences" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Water Rights Licences" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -68,26 +67,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Point of well diversion</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="69">
   <si>
     <t xml:space="preserve">Surface water</t>
   </si>
@@ -122,18 +107,15 @@
     <t xml:space="preserve">POD</t>
   </si>
   <si>
-    <t xml:space="preserve">PWD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PG</t>
-  </si>
-  <si>
     <t xml:space="preserve">Source</t>
   </si>
   <si>
     <t xml:space="preserve">Water licences (public)</t>
   </si>
   <si>
+    <t xml:space="preserve">{ d.licences_count_pod }</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://catalogue.data.gov.bc.ca/dataset/water-rights-licences-public</t>
   </si>
   <si>
@@ -149,32 +131,165 @@
     <t xml:space="preserve">{ d.drainage_area }</t>
   </si>
   <si>
-    <t xml:space="preserve">Median elevation:</t>
+    <t xml:space="preserve">Median elevation (mASL):</t>
   </si>
   <si>
     <t xml:space="preserve">{ d.median_elevation }</t>
   </si>
   <si>
-    <t xml:space="preserve">Glacial coverage:</t>
+    <t xml:space="preserve">Glacial coverage (%):</t>
   </si>
   <si>
     <t xml:space="preserve">{ d.glacial_coverage }</t>
   </si>
   <si>
-    <t xml:space="preserve">Annual precipitation:</t>
+    <t xml:space="preserve">Annual precipitation (mm):</t>
   </si>
   <si>
     <t xml:space="preserve">{ d.annual_precipitation }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Rights Licences in Watershed: { d.watershed_name }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Methodology:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All water licences of subtype POD that are contained by the watershed boundary.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warning:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licences that fall outside the boundary are not included. Incorrect boundary or incorrect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">licence locations may result in missing licences. You must verify that all licences relevant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to the search area have been accounted for.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POD Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">File number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licence number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POD status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Licence status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POD subtype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Priority date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expiry date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purpose use code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Purpose use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity (m3/year)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydraulic connectivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Primary licensee name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.licences[i].POD_NUMBER }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.licences[i].FILE_NUMBER }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.licences[i].LICENCE_NUMBER }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.licences[i].POD_STATUS }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.licences[i].LICENCE_STATUS }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.licences[i].PRIORITY_DATE }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.licences[i].EXPIRY_DATE }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.licences[i].PURPOSE_USE_CODE }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.licences[i].PURPOSE_USE }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.licences[i].SOURCE_NAME }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.licences[i].QUANTITY }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.licences[i].QUANTITY_UNITS }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.licences[i].qty_m3_yr }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.licences[i].HYDRAULIC_CONNECTIVITY }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.licences[i].PRIMARY_LICENSEE_NAME }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.licences[i].LATITUDE }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.licences[i].LONGITUDE }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.licences[i+1].POD_NUMBER }</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -222,6 +337,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -235,6 +358,19 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -263,7 +399,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -290,8 +426,11 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -308,8 +447,28 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
@@ -317,6 +476,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Excel Built-in Heading 1" xfId="20"/>
+    <cellStyle name="Heading 1" xfId="21"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -386,10 +546,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -456,7 +616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>5</v>
       </c>
@@ -466,63 +626,71 @@
       <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="3" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="B11" s="0" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="C11" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="0" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+      <c r="B12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="0" t="s">
-        <v>17</v>
+    </row>
+    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="0" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+      <c r="B16" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -541,37 +709,214 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="O21" activeCellId="0" sqref="O21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.63"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="O15" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="P15" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q15" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="R15" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
add basic model info to spreadsheet
</commit_message>
<xml_diff>
--- a/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
+++ b/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Water Rights Licences" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Runoff and Streamflow Models" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="84">
   <si>
     <t xml:space="preserve">Surface water</t>
   </si>
@@ -279,6 +280,51 @@
   </si>
   <si>
     <t xml:space="preserve">{ d.licences[i+1].POD_NUMBER }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runoff and Streamflow Models</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal Annual Runoff Isolines (1961 - 1990) – Historical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://catalogue.data.gov.bc.ca/dataset/hydrology-normal-annual-runoff-isolines-1961-1990-historical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydrology: Hydrometric Watersheds Normalized Runoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://catalogue.data.gov.bc.ca/dataset/hydrology-hydrometric-watershed-boundaries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Coast Stewardship Baseline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.status }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean Annual Discharge (estimates):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAD (m3/s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20% MAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10% MAD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runoff isolines:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydrometric normalized runoff:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Coast Stewardship Baseline:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Coast Stewardship Baseline Data</t>
   </si>
 </sst>
 </file>
@@ -289,7 +335,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -311,6 +357,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -358,19 +411,6 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -423,27 +463,27 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -455,16 +495,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -475,8 +511,8 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Excel Built-in Heading 1" xfId="20"/>
-    <cellStyle name="Heading 1" xfId="21"/>
+    <cellStyle name="Heading 1 1" xfId="20"/>
+    <cellStyle name="Excel Built-in Heading 1" xfId="21"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -548,11 +584,11 @@
   </sheetPr>
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.578125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.17"/>
@@ -712,32 +748,40 @@
   <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O21" activeCellId="0" sqref="O21"/>
+      <selection pane="topLeft" activeCell="O25" activeCellId="0" sqref="O25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="19.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.63"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+    <row r="1" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -904,16 +948,182 @@
       <c r="P15" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="Q15" s="8" t="s">
+      <c r="Q15" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="R15" s="8" t="s">
+      <c r="R15" s="4" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.24"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <f aca="false">B13*0.2</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <f aca="false">B13*0.1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <f aca="false">B14*0.2</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <f aca="false">B14*0.1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <f aca="false">B15*0.2</f>
+        <v>0</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <f aca="false">B15*0.1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more model data in spreadsheet
</commit_message>
<xml_diff>
--- a/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
+++ b/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="113">
   <si>
     <t xml:space="preserve">Surface water</t>
   </si>
@@ -243,6 +243,9 @@
     <t xml:space="preserve">{ d.licences[i].LICENCE_STATUS }</t>
   </si>
   <si>
+    <t xml:space="preserve">{ d.licences[i].POD_SUBTYPE }</t>
+  </si>
+  <si>
     <t xml:space="preserve">{ d.licences[i].PRIORITY_DATE }</t>
   </si>
   <si>
@@ -303,7 +306,7 @@
     <t xml:space="preserve">{ d.scsb2016_output.status }</t>
   </si>
   <si>
-    <t xml:space="preserve">Mean Annual Discharge (estimates):</t>
+    <t xml:space="preserve">Mean Annual Discharge (estimated):</t>
   </si>
   <si>
     <t xml:space="preserve">MAD (m3/s)</t>
@@ -318,13 +321,97 @@
     <t xml:space="preserve">Runoff isolines:</t>
   </si>
   <si>
+    <t xml:space="preserve">{ d.runoff_isoline_discharge_m3s }</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hydrometric normalized runoff:</t>
   </si>
   <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
     <t xml:space="preserve">South Coast Stewardship Baseline:</t>
   </si>
   <si>
+    <t xml:space="preserve">{ d.scsb2016_output.mad }</t>
+  </si>
+  <si>
     <t xml:space="preserve">South Coast Stewardship Baseline Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly discharge (m3/s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.1 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.2 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.3 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.4 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.5 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.6 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.7 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.8 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.9 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.10 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.11 }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.12 }</t>
   </si>
 </sst>
 </file>
@@ -747,8 +834,8 @@
   </sheetPr>
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O25" activeCellId="0" sqref="O25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N15" activeCellId="0" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -922,42 +1009,42 @@
         <v>57</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="P15" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -976,21 +1063,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.69"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1008,32 +1097,32 @@
     </row>
     <row r="3" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1070,60 +1159,146 @@
     </row>
     <row r="12" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="0" t="e">
         <f aca="false">B13*0.2</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="0" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D13" s="0" t="e">
         <f aca="false">B13*0.1</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="C14" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="0" t="e">
         <f aca="false">B14*0.2</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="0" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D14" s="0" t="e">
         <f aca="false">B14*0.1</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="C15" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="0" t="e">
         <f aca="false">B15*0.2</f>
-        <v>0</v>
-      </c>
-      <c r="D15" s="0" t="n">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D15" s="0" t="e">
         <f aca="false">B15*0.1</f>
-        <v>0</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>83</v>
+        <v>87</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="M19" s="0" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
handle empty values for scsb model monthly values
</commit_message>
<xml_diff>
--- a/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
+++ b/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -381,40 +381,40 @@
     <t xml:space="preserve">Monthly discharge (m3/s)</t>
   </si>
   <si>
-    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.1:round(2) }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.2:round(2) }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.3:round(2) }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.4:round(2) }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.5:round(2) }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.6:round(2) }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.7:round(2) }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.8:round(2) }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.9:round(2) }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.10:round(2) }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.11:round(2) }</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.12:round(2) }</t>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.1.model_result:ifEmpty( ):round(2) }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.2.model_result:ifEmpty( ):round(2) }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.3.model_result:ifEmpty( ):round(2) }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.4.model_result:ifEmpty( ):round(2) }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.5.model_result:ifEmpty( ):round(2) }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.6.model_result:ifEmpty( ):round(2) }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.7.model_result:ifEmpty( ):round(2) }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.8.model_result:ifEmpty( ):round(2) }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.9.model_result:ifEmpty( ):round(2) }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.10.model_result:ifEmpty( ):round(2) }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.11.model_result:ifEmpty( ):round(2) }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.monthly_discharge.12.model_result:ifEmpty( ):round(2) }</t>
   </si>
 </sst>
 </file>
@@ -674,7 +674,7 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -1062,10 +1062,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B35" activeCellId="0" sqref="B35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1281,6 +1281,7 @@
         <v>113</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
update licence excel tabs
</commit_message>
<xml_diff>
--- a/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
+++ b/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
@@ -9,8 +9,9 @@
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Water Rights Licences" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Runoff and Streamflow Models" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Water Rights Licences (Active)" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Water Rights Licences (Inactive" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Runoff and Streamflow Models" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="139">
   <si>
     <t xml:space="preserve">Watershed Analysis – Summary</t>
   </si>
@@ -262,6 +263,75 @@
   </si>
   <si>
     <t xml:space="preserve">{ d.licences[i+1].POD_NUMBER }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water Rights Licences in Watershed (Inactive/Expired/Cancelled)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All inactive water licences of subtype POD that are contained by the watershed boundary.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The dataset is filtered on POD_STATUS and LICENCE_STATUS properties. This table contains only POD records </t>
+  </si>
+  <si>
+    <t xml:space="preserve">with a status of ‘Inactive’, ‘Cancelled’, ‘Expired’, or ‘Abandoned’.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i].POD_NUMBER }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i].FILE_NUMBER }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i].LICENCE_NUMBER }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i].POD_STATUS }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i].LICENCE_STATUS }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i].POD_SUBTYPE }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i].PRIORITY_DATE }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i].EXPIRY_DATE }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i].PURPOSE_USE_CODE }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i].PURPOSE_USE }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i].SOURCE_NAME }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i].QUANTITY }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i].QUANTITY_UNITS }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i].qty_m3_yr }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i].HYDRAULIC_CONNECTIVITY }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i].PRIMARY_LICENSEE_NAME }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i].LATITUDE }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i].LONGITUDE }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.inactive_licences[i+1].POD_NUMBER }</t>
   </si>
   <si>
     <t xml:space="preserve">Runoff and Streamflow Models</t>
@@ -632,7 +702,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -642,7 +712,7 @@
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.62890625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.64453125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.17"/>
@@ -800,17 +870,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.40234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.41796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.07"/>
@@ -857,165 +927,165 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>33</v>
+      <c r="A11" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="P14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q14" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="R14" s="3" t="s">
-        <v>52</v>
+      <c r="A14" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B17" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C17" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D17" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E17" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F17" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="G17" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="H17" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="I15" s="0" t="s">
+      <c r="I17" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="J15" s="0" t="s">
+      <c r="J17" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="K15" s="0" t="s">
+      <c r="K17" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="L15" s="0" t="s">
+      <c r="L17" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="M15" s="0" t="s">
+      <c r="M17" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="N15" s="0" t="s">
+      <c r="N17" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="O15" s="0" t="s">
+      <c r="O17" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="P15" s="0" t="s">
+      <c r="P17" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="Q15" s="4" t="s">
+      <c r="Q17" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="R15" s="4" t="s">
+      <c r="R17" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1031,7 +1101,227 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:R18"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="M17" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="N17" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="O17" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="P17" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1041,7 +1331,7 @@
       <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.38671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.40234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.26"/>
@@ -1051,7 +1341,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1069,23 +1359,23 @@
     </row>
     <row r="3" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="34.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1095,7 +1385,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>78</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1103,7 +1393,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1119,7 +1409,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1127,7 +1417,7 @@
         <v>24</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1137,34 +1427,34 @@
     </row>
     <row r="13" customFormat="false" ht="26.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>87</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1174,84 +1464,84 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>102</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>108</v>
+        <v>131</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>110</v>
+        <v>133</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>111</v>
+        <v>134</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>113</v>
+        <v>136</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
fix spreadsheet tab name
</commit_message>
<xml_diff>
--- a/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
+++ b/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
@@ -712,7 +712,7 @@
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.64453125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.17"/>
@@ -880,7 +880,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.41796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.07"/>
@@ -1111,7 +1111,7 @@
       <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1151,7 +1151,6 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>30</v>
@@ -1331,7 +1330,7 @@
       <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.40234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.41796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.26"/>

</xml_diff>

<commit_message>
set excel starting sheet
</commit_message>
<xml_diff>
--- a/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
+++ b/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -708,11 +708,11 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6953125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.17"/>
@@ -876,11 +876,11 @@
   </sheetPr>
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.4765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.07"/>
@@ -1111,7 +1111,7 @@
       <selection pane="topLeft" activeCell="D29" activeCellId="0" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.38671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.40234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="26.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1330,7 +1330,7 @@
       <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.26"/>

</xml_diff>

<commit_message>
Add Hydro data to summary
Updated the excel template to display Hydrometric station data on the summary page.
</commit_message>
<xml_diff>
--- a/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
+++ b/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chriswalsh/Desktop/Projects/wally/backend/api/v1/watersheds/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7493FF-A6E8-EE42-97BE-66CE786CF33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED10303-65D6-CB40-B4BD-F56FAEC94B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3020" yWindow="2120" windowWidth="27180" windowHeight="16580" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5620" yWindow="2740" windowWidth="27180" windowHeight="16580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="221">
   <si>
     <t>Watershed Analysis – Summary</t>
   </si>
@@ -482,18 +482,9 @@
     <t>WALLY %MAD</t>
   </si>
   <si>
-    <t>WSC $MAD</t>
-  </si>
-  <si>
     <t>WSC MAD</t>
   </si>
   <si>
-    <t>Sanity Check!</t>
-  </si>
-  <si>
-    <t>WSC MMD TEXT VALUE</t>
-  </si>
-  <si>
     <t>{ d.scsb2016_output.monthly_discharge.1.model_result:round(2) }</t>
   </si>
   <si>
@@ -606,6 +597,135 @@
   </si>
   <si>
     <t>{ d.baseLineMean.11:round(2) }</t>
+  </si>
+  <si>
+    <t>Low 7Q2 (m3)</t>
+  </si>
+  <si>
+    <t>Mean Annual Runoff (L/S/km2)</t>
+  </si>
+  <si>
+    <t>{ d.scsb2016_output.mar.model_result:round(2) }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ d.scsb2016_output.7q2.model_result:round(2) } </t>
+  </si>
+  <si>
+    <t>Dry 7Q10 (m3/s)</t>
+  </si>
+  <si>
+    <t>{ d.scsb2016_output.s7q10.model_result:round(2) }</t>
+  </si>
+  <si>
+    <t>Station Name</t>
+  </si>
+  <si>
+    <t>Station Number</t>
+  </si>
+  <si>
+    <t>MAD</t>
+  </si>
+  <si>
+    <t>%MAD</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>P90</t>
+  </si>
+  <si>
+    <t>{ d.hydrometric_stations.0.properties.name }</t>
+  </si>
+  <si>
+    <t>{ d.hydrometric_stations.0.id }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WSC MMD </t>
+  </si>
+  <si>
+    <t>Hydrometric Station MMD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMD </t>
+  </si>
+  <si>
+    <t>WSC %MAD</t>
+  </si>
+  <si>
+    <t>Hydrometric Station</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.0.p10:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.1.p10:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.2.p10:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.3.p10:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.4.p10:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.5.p10:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.6.p10:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.7.p10:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.8.p10:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.9.p10:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.10.p10:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.11.p10:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.0.p90:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.1.p90:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.2.p90:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.3.p90:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.4.p90:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.5.p90:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.6.p90:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.7.p90:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.8.p90:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.9.p90:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.10.p90:round(2) }</t>
+  </si>
+  <si>
+    <t>{ d.flowData.months.11.p90:round(2) }</t>
   </si>
 </sst>
 </file>
@@ -652,12 +772,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -697,11 +816,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Heading 1" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
@@ -1086,17 +1205,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.1640625" customWidth="1"/>
-    <col min="5" max="5" width="64.33203125" customWidth="1"/>
+    <col min="1" max="1" width="50.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="13" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1229,11 +1347,271 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B18" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B31" s="5"/>
+    <row r="23" spans="1:13" ht="30" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>184</v>
+      </c>
+      <c r="B25" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>185</v>
+      </c>
+      <c r="B26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>186</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>194</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>187</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>188</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="L32" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>189</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>220</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1688,8 +2066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1722,7 +2100,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>96</v>
       </c>
       <c r="B3" t="s">
@@ -1730,7 +2108,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>98</v>
       </c>
       <c r="B4" t="s">
@@ -1738,7 +2116,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="33.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1788,9 +2166,6 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
-      <c r="B12" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="13" spans="1:9" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
@@ -1826,10 +2201,10 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>140</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>168</v>
+        <v>139</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -1878,7 +2253,7 @@
         <v>126</v>
       </c>
       <c r="B19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C19" t="s">
         <v>127</v>
@@ -1918,123 +2293,123 @@
       <c r="A20" t="s">
         <v>138</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="F20" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="G20" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="H20" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="I20" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="J20" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="K20" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="I20" s="7" t="s">
+      <c r="L20" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="J20" s="7" t="s">
+      <c r="M20" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="L20" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="M20" s="7" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>142</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="E21" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="I21" s="7" t="s">
+      <c r="F21" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="G21" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="K21" s="7" t="s">
+      <c r="H21" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="L21" s="7" t="s">
+      <c r="I21" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="M21" s="7" t="s">
+      <c r="J21" s="6" t="s">
         <v>156</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>139</v>
-      </c>
-      <c r="B22" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="F22" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="G22" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="H22" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="I22" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="J22" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="K22" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="I22" s="7" t="s">
+      <c r="L22" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="M22" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="K22" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="L22" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="M22" s="7" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Drainage Area to Export
Added the gross drainage area for Hydrometric station to the excel export on the worksheets summary page.
</commit_message>
<xml_diff>
--- a/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
+++ b/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chriswalsh/Desktop/Projects/wally/backend/api/v1/watersheds/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED10303-65D6-CB40-B4BD-F56FAEC94B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33572669-5F45-9648-8E2D-CBCCB617B0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5620" yWindow="2740" windowWidth="27180" windowHeight="16580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="223">
   <si>
     <t>Watershed Analysis – Summary</t>
   </si>
@@ -726,13 +726,19 @@
   </si>
   <si>
     <t>{ d.flowData.months.11.p90:round(2) }</t>
+  </si>
+  <si>
+    <t>Gross Drainage Area</t>
+  </si>
+  <si>
+    <t>{ d.hydrometric_stations.0.properties.drainage_area_gross:round(2) }</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -778,6 +784,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF44546A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF44546A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -810,7 +832,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyProtection="1"/>
@@ -821,6 +843,8 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Heading 1" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
@@ -1208,13 +1232,13 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="6.5" customWidth="1"/>
+    <col min="2" max="13" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1385,7 +1409,7 @@
     </row>
     <row r="24" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="3" t="s">
         <v>184</v>
       </c>
       <c r="B25" t="s">
@@ -1393,64 +1417,72 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" s="3" t="s">
         <v>185</v>
       </c>
       <c r="B26" t="s">
         <v>191</v>
       </c>
     </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>186</v>
+      <c r="A28" s="3" t="s">
+        <v>221</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="E29" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="H29" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="I29" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="J29" s="3" t="s">
+      <c r="J29" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="K29" s="3" t="s">
+      <c r="K29" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="L29" s="3" t="s">
+      <c r="L29" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="M29" s="3" t="s">
+      <c r="M29" s="9" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="30" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>194</v>
       </c>
       <c r="B30" s="6" t="s">
@@ -1491,7 +1523,7 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="A31" s="3" t="s">
         <v>187</v>
       </c>
       <c r="B31" s="6" t="s">
@@ -1532,7 +1564,7 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="A32" s="3" t="s">
         <v>188</v>
       </c>
       <c r="B32" s="6" t="s">
@@ -1573,7 +1605,7 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="A33" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B33" s="6" t="s">

</xml_diff>

<commit_message>
Debug missing flow years
Local instance has no values for the years of reporting for hydrometric stations. This update should add the output to the excel doc for the missing fields. If they are available in dev instance of app.
</commit_message>
<xml_diff>
--- a/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
+++ b/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chriswalsh/Desktop/Projects/wally/backend/api/v1/watersheds/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33572669-5F45-9648-8E2D-CBCCB617B0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA31D54-9400-144A-AC23-C9CDA77B39F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5620" yWindow="2740" windowWidth="27180" windowHeight="16580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="229">
   <si>
     <t>Watershed Analysis – Summary</t>
   </si>
@@ -732,6 +732,24 @@
   </si>
   <si>
     <t>{ d.hydrometric_stations.0.properties.drainage_area_gross:round(2) }</t>
+  </si>
+  <si>
+    <t>Flow years</t>
+  </si>
+  <si>
+    <t>{ d.hydrometric_stations.0.flow_years }</t>
+  </si>
+  <si>
+    <t>{ d.hydrometric_stations.0.real_time }</t>
+  </si>
+  <si>
+    <t>Real time?</t>
+  </si>
+  <si>
+    <t>Level years</t>
+  </si>
+  <si>
+    <t>{ d.hydrometric_stations.0.level_years }</t>
   </si>
 </sst>
 </file>
@@ -1229,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1643,6 +1661,30 @@
       </c>
       <c r="M33" s="6" t="s">
         <v>220</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Normailze Quantity Seconds
Added the logic for converting varying quantities to a normalized standard  (in seconds).

Used this to add the data to the appropriate pages in the excel document export.

Removed more debugging previously added to view logs in dev environment.
</commit_message>
<xml_diff>
--- a/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
+++ b/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chriswalsh/Desktop/Projects/wally/backend/api/v1/watersheds/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176C232F-D055-6944-8B39-282C735C70BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CE8A95-18B3-594D-A4D0-947B0AB3E2D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="2740" windowWidth="27180" windowHeight="16580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4720" yWindow="3240" windowWidth="27180" windowHeight="16580" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="227">
   <si>
     <t>Watershed Analysis – Summary</t>
   </si>
@@ -735,6 +735,15 @@
   </si>
   <si>
     <t>P90 (m3/s)</t>
+  </si>
+  <si>
+    <t>Quantity (m3/second)</t>
+  </si>
+  <si>
+    <t>{ d.licences[i].qty_m3_second }</t>
+  </si>
+  <si>
+    <t>{ d.inactive_licences[i].qty_m3_second }</t>
   </si>
 </sst>
 </file>
@@ -1234,7 +1243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
@@ -1673,10 +1682,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1694,11 +1703,12 @@
     <col min="11" max="11" width="12.33203125" customWidth="1"/>
     <col min="13" max="13" width="13.33203125" customWidth="1"/>
     <col min="14" max="14" width="17.1640625" customWidth="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
-    <col min="16" max="16" width="20.6640625" customWidth="1"/>
+    <col min="15" max="15" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20" customWidth="1"/>
+    <col min="17" max="17" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -1711,67 +1721,67 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
@@ -1815,19 +1825,22 @@
         <v>48</v>
       </c>
       <c r="O16" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="P16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="P16" s="3" t="s">
+      <c r="Q16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="Q16" s="3" t="s">
+      <c r="R16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="R16" s="3" t="s">
+      <c r="S16" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -1871,19 +1884,22 @@
         <v>66</v>
       </c>
       <c r="O17" t="s">
+        <v>225</v>
+      </c>
+      <c r="P17" t="s">
         <v>67</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>68</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>69</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>71</v>
       </c>
@@ -1900,15 +1916,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:R18"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="14" max="14" width="17.83203125" customWidth="1"/>
+    <col min="15" max="15" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -1921,72 +1941,72 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>35</v>
       </c>
@@ -2030,19 +2050,22 @@
         <v>48</v>
       </c>
       <c r="O16" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="P16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="P16" s="3" t="s">
+      <c r="Q16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="Q16" s="3" t="s">
+      <c r="R16" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="R16" s="3" t="s">
+      <c r="S16" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -2086,19 +2109,22 @@
         <v>89</v>
       </c>
       <c r="O17" t="s">
+        <v>226</v>
+      </c>
+      <c r="P17" t="s">
         <v>90</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>91</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>92</v>
       </c>
-      <c r="R17" t="s">
+      <c r="S17" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
Added Fish Observation data
Added fish observation data to the summary page of the export

Created and styled a Fish summary page.

Formatted excel document to work with new data.
</commit_message>
<xml_diff>
--- a/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
+++ b/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chriswalsh/Desktop/Projects/wally/backend/api/v1/watersheds/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CE8A95-18B3-594D-A4D0-947B0AB3E2D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C8A4E6-9C80-FD40-997F-E458BCC41AE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4720" yWindow="3240" windowWidth="27180" windowHeight="16580" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2960" yWindow="2060" windowWidth="27180" windowHeight="16580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Active Water Rights Licences" sheetId="2" r:id="rId2"/>
-    <sheet name="Inactive Water Rights Licences" sheetId="3" r:id="rId3"/>
-    <sheet name="Runoff and Streamflow Models" sheetId="4" r:id="rId4"/>
+    <sheet name="Fish Observation Data" sheetId="5" r:id="rId2"/>
+    <sheet name="Active Water Rights Licences" sheetId="2" r:id="rId3"/>
+    <sheet name="Inactive Water Rights Licences" sheetId="3" r:id="rId4"/>
+    <sheet name="Runoff and Streamflow Models" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="242">
   <si>
     <t>Watershed Analysis – Summary</t>
   </si>
@@ -744,6 +745,51 @@
   </si>
   <si>
     <t>{ d.inactive_licences[i].qty_m3_second }</t>
+  </si>
+  <si>
+    <t>Watershed Fish Observations</t>
+  </si>
+  <si>
+    <t>Fish Species</t>
+  </si>
+  <si>
+    <t>Observation Count</t>
+  </si>
+  <si>
+    <t>Life Stages Observed</t>
+  </si>
+  <si>
+    <t>First Observation Date</t>
+  </si>
+  <si>
+    <t>Last Observation Date</t>
+  </si>
+  <si>
+    <t>{ d.fish_data[i].POD_NUMBER }</t>
+  </si>
+  <si>
+    <t>Pod Number</t>
+  </si>
+  <si>
+    <t>{ d.fish_data[i].species }</t>
+  </si>
+  <si>
+    <t>{ d.fish_data[i].count }</t>
+  </si>
+  <si>
+    <t>{ d.fish_data[i].observation_date_min }</t>
+  </si>
+  <si>
+    <t>{ d.fish_data[i].observation_date_max }</t>
+  </si>
+  <si>
+    <t>{ d.fish_data[i+1].POD_NUMBER }</t>
+  </si>
+  <si>
+    <t>{ d.fish_data[i].life_stages }</t>
+  </si>
+  <si>
+    <t>{ d.fish_data[i+1].species }</t>
   </si>
 </sst>
 </file>
@@ -1241,10 +1287,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1665,13 +1711,55 @@
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
-      <c r="B36" s="6"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-      <c r="B37" s="6"/>
+    <row r="36" spans="1:13" ht="30" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>228</v>
+      </c>
+      <c r="B37" t="s">
+        <v>229</v>
+      </c>
+      <c r="C37" t="s">
+        <v>231</v>
+      </c>
+      <c r="D37" t="s">
+        <v>232</v>
+      </c>
+      <c r="E37" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>235</v>
+      </c>
+      <c r="B38" t="s">
+        <v>236</v>
+      </c>
+      <c r="C38" t="s">
+        <v>237</v>
+      </c>
+      <c r="D38" t="s">
+        <v>238</v>
+      </c>
+      <c r="E38" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>241</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1681,11 +1769,86 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D30089E-6F35-4442-871D-FD41C5FE1AA1}">
+  <dimension ref="A1:K4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="18.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" ht="30" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D2" t="s">
+        <v>231</v>
+      </c>
+      <c r="E2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D3" t="s">
+        <v>237</v>
+      </c>
+      <c r="E3" t="s">
+        <v>238</v>
+      </c>
+      <c r="F3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1914,12 +2077,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2139,7 +2302,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M22"/>
   <sheetViews>

</xml_diff>

<commit_message>
Handling of incomplete data
Added try catch block to handle hydrometric stations with incomplete data.
</commit_message>
<xml_diff>
--- a/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
+++ b/backend/api/v1/watersheds/templates/SurfaceWater.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chriswalsh/Desktop/Projects/wally/backend/api/v1/watersheds/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF818F3-D4B0-1943-9327-0771B624CAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF7B689-F4C5-8444-9188-C9637A8FF5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="2060" windowWidth="27180" windowHeight="16580" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2960" yWindow="2060" windowWidth="27180" windowHeight="16580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -1283,8 +1283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1858,7 +1858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>

</xml_diff>